<commit_message>
Minor updates to ProjectTemplate
</commit_message>
<xml_diff>
--- a/ProjectEstimationTemplate.xlsx
+++ b/ProjectEstimationTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jhash/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB614247-EA3C-6346-A39C-4DE250663253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92020CB3-112B-F146-A58D-5DE6C9F172A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1480" yWindow="500" windowWidth="32120" windowHeight="20500" activeTab="1" xr2:uid="{1B655C53-9223-9C48-865C-9AC28ECBCECA}"/>
+    <workbookView xWindow="1480" yWindow="500" windowWidth="32120" windowHeight="20500" xr2:uid="{1B655C53-9223-9C48-865C-9AC28ECBCECA}"/>
   </bookViews>
   <sheets>
     <sheet name="Guide" sheetId="3" r:id="rId1"/>
@@ -1308,7 +1308,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5EC6CCE2-EB73-494E-8587-024C1544A406}">
   <dimension ref="B1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -1406,11 +1406,11 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK153"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="9" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H2" sqref="H2"/>
+      <selection pane="bottomRight" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>